<commit_message>
Actualizacion del documento excel, hallazgos, papeles de trabajo y debilidades 1 y 2 fueron completadas
</commit_message>
<xml_diff>
--- a/Actividad04/Actividad04_Grupo14.xlsx
+++ b/Actividad04/Actividad04_Grupo14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pamel\Documents\Universidad\CuatrimestreI2025\Auditoría de Sistemas\Auditoria-ISW1012-Actividades\Actividad04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE67E887-B03B-4D30-9738-A79B21491B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303A0DD6-28BA-49CC-B8FA-0B6A506AED24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{A49F3D99-767D-41B4-B62A-39BE75E974FA}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="121">
   <si>
     <t>#</t>
   </si>
@@ -359,142 +359,6 @@
   </si>
   <si>
     <t>Fallos en la creación de reportes debido a la falta de accesibilidad o integridad de la información.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1- Identificación del criterio:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
- Una llave foránea debe existir en una tabla si la tabla tiene una columna con el nombre definido con la siguiente nomenclatura: id_&lt;nombre tabla referenciada&gt;.                                                                                                                                                                                                                                                                                               Prococedemos a realizar una consulta para verificar la existencia de las llaves foráneas,</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">2- Consulta SQL utilizada:           </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                           WITH columns_with_id_convention AS (
-    SELECT 
-        table_schema,
-        table_name,
-        column_name,
-        REPLACE(column_name, 'id_', '') AS referenced_table_name
-    FROM information_schema.columns
-    WHERE column_name LIKE 'id_%'
-    AND table_schema = 'actividad02'
-),
-foreign_key_info AS (
-    SELECT 
-        tc.table_schema,
-        tc.table_name,
-        kcu.column_name,
-        ccu.table_name AS referenced_table_name
-    FROM information_schema.table_constraints tc
-    JOIN information_schema.key_column_usage kcu
-        ON tc.constraint_name = kcu.constraint_name
-        AND tc.table_schema = kcu.table_schema
-        AND tc.table_name = kcu.table_name
-    JOIN information_schema.constraint_column_usage ccu
-        ON tc.constraint_name = ccu.constraint_name
-        AND tc.table_schema = ccu.table_schema
-    WHERE tc.constraint_type = 'FOREIGN KEY'
-    AND tc.table_schema = 'actividad02' -- Filter for actividad02 schema
-)
-SELECT 
-    c.table_schema AS ESQUEMA,
-    c.table_name AS NOMBRE_DE_TABLA,
-    c.column_name AS COLUMNA_CON_ID,
-    fk.referenced_table_name AS TABLA_REFERENCIADA,
-    CASE 
-        WHEN fk.referenced_table_name IS NOT NULL THEN 'Correcto'
-        ELSE 'No tiene llave foranea registrada'
-    END AS VALIDACION_FK
-FROM columns_with_id_convention c
-LEFT JOIN foreign_key_info fk
-    ON c.table_schema = fk.table_schema
-    AND c.table_name = fk.table_name
-    AND c.column_name = fk.column_name
-    AND c.referenced_table_name = fk.referenced_table_name
-WHERE fk.referenced_table_name IS NULL
-ORDER BY VALIDACION_FK DESC;</t>
-    </r>
-  </si>
-  <si>
-    <t>Se obtiene el resultado donde hay incosistencias con la  tabla actividad02.estudiantes, donde no se presenta una llave foránea a pesar de tener una columna para ella.       
-Se adjunta resultado obtenido Referencia 003</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">3-Análisis de los resultados:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Se detecta una inconsistencia en la nomenclatura de las llaves foráneas, donde el 20% de las columnas que deberían de tener llaves foráneas, no la tienen. Esto incumple la integridad de los datos y las buenas prácticas. Se recomienda agregarle una llave foránea a la columna que la tiene por diseño.</t>
-    </r>
-  </si>
-  <si>
-    <t>Referencia003</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2- Consulta SQL utilizada:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                                                                                 </t>
-    </r>
   </si>
   <si>
     <r>
@@ -531,34 +395,11 @@
     <t>Construya el hallazgo de la debilidad identificadas en los papeles de trabajo: condición, causa, efecto, criterio. Realice una posible recomendación para subsanar la debilidad encontrada (1 hallazgo por debilidad y que corresponda a un papel de trabajo)</t>
   </si>
   <si>
-    <t>Se identificaron llaves primarias en el esquema actividad02 que no cumplen con la nomenclatura estándar definida, específicamente las llaves foráneas en las tablas cursos, estudiantes y personas.</t>
-  </si>
-  <si>
-    <t>El sistema no ha implementado correctamente la nomenclatura definida para las llaves primarias. Esto puede deberse a un error en la aplicación de los estándares o a una falta de conocimiento de las reglas de nomenclatura por parte de los desarrolladores de la base de datos.</t>
-  </si>
-  <si>
-    <t>Dificultad en la identificación de llaves primarias en las tablas.
-Incremento en la complejidad del mantenimiento y documentación de la base de datos.
-Incumplimiento de estándares que pueden generar confusión en futuros desarrollos.</t>
-  </si>
-  <si>
-    <t>Artículo I Insiso 1 - Llaves primarias</t>
-  </si>
-  <si>
-    <t>1- Renombrar las llaves primarias de las tablas cursos, estudiantes y personas para que cumplan con el formato establecido de pk_&lt;nombre_tabla&gt;
-2- Realizar auditorías periódicas para asegurar el cumplimiento de los estándares de nomenclatura.
-3- Capacitar a los desarrolladores sobre las reglas de nomenclatura de las llaves primarias para evitar repeticiones del error.</t>
-  </si>
-  <si>
-    <t>Se obtiene el resultado donde hay incosistencias con la  tabla proyecto.estudiantes, donde no se presenta una llave foránea a pesar de tener una columna para ella.
-Se adjunta resultado obtenido Referencia 001</t>
-  </si>
-  <si>
     <t>Referencia001</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">3-Análisis de los resultados:
+      <t xml:space="preserve">4 -  Documentación de inconsistencias:
 </t>
     </r>
     <r>
@@ -570,6 +411,297 @@
         <scheme val="minor"/>
       </rPr>
       <t>Se detecta una inconsistencia en la nomenclatura del asunto de los tiquetes de la prueba de calidad en la tabla ticket, donde el 50% de los nombres de tiquetes tienen un formato incorrecto. Esto incumple las reglas de nomenclatura establecidas por la empresa. Se recomienda cambiarle el nombre a los tiquetes que no cumplen las reglas y agregar medidas para que no se incumplan en el futuro.</t>
+    </r>
+  </si>
+  <si>
+    <t>Referencia002</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2- Consulta SQL utilizada:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WITH tickets_information AS (
+    SELECT 
+        t.id,
+        t.asunto AS asunto_actual,
+        p.codigo AS codigo,
+        '[' || p.codigo || ']Pruebas de Calidad' AS asunto_esperado
+    FROM proyecto.ticket t
+    LEFT JOIN proyecto.proyecto p  
+        ON t.asunto LIKE '%[' || p.codigo || ']%' 
+        OR t.asunto LIKE '%(' || p.codigo || ')%' 
+    WHERE 
+        LOWER(t.asunto) LIKE '%prueba%' 
+        AND LOWER(t.asunto) LIKE '%calidad%'
+)
+SELECT 
+    current_database() AS base_de_datos,
+    tbl.table_schema AS schema,
+    tbl.table_name AS tabla,
+    ti.id,
+    ti.asunto_actual,
+    ti.asunto_esperado,
+    'No coincide' AS estado_de_validacion,
+    NOW() AS fecha_de_validacion
+FROM information_schema.tables AS tbl
+JOIN tickets_information AS ti 
+    ON tbl.table_name = 'ticket'
+WHERE 
+    tbl.table_schema = 'proyecto'
+    AND ti.asunto_actual != ti.asunto_esperado
+    OR ti.asunto_esperado IS NULL;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 - Análisis de Información:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Se obtiene un resultado en el que una  de las leyendas registradas para la prueba de calidad en la tabla "ticket" no coincide con el formato establecido en el diseño, pues usa paréntesis en lugar de corchetes al escribir el código de proyecto.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Se adjunta resultado obtenido Referencia 001</t>
+    </r>
+  </si>
+  <si>
+    <t>El formato de las leyendas no coincide con aquel impuesto en la nomeclatura diseñada.</t>
+  </si>
+  <si>
+    <t>Existe un proyecto marcado como finalizado que no tiene las 4 secciones obligatorias para considerarse así.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1- Identificación del criterio:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ En el procedimiento Proyectos, Sección Documentación, Artículo VI - Responsabilidades, Inciso 1: Todo proyecto finalizado debe contener la documentacion de cada uno de los procesos de desarrollo en el sistema: requerimientos, pruebas de calidad y usuarios y pase a produccion.
+Se procede a realizar una consulta para verificar la existencia de todos los procesos para los proyectos finalizados,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2- Consulta SQL utilizada:           </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                           
+WITH project_tickets AS (
+    SELECT 
+        p.codigo AS proyecto_codigo,
+        p.nombre AS proyecto_nombre,
+        p.estado AS proyecto_estado,
+        t.id AS ticket_id,
+        t.servicio,
+        t.asunto,
+        t.responsable,
+        t.fecha_creacion,
+        CASE 
+            WHEN LOWER(t.asunto) LIKE '%historias de usuario%' THEN 'Historias de Usuario'
+            WHEN LOWER(t.asunto) LIKE '%pruebas de calidad%' THEN 'Pruebas de Calidad'
+            WHEN LOWER(t.asunto) LIKE '%pruebas de usuario%' THEN 'Pruebas de Usuario'
+            WHEN LOWER(t.asunto) LIKE '%pase a produccion%' OR LOWER(t.asunto) LIKE '%pase a producción%' THEN 'Pase a Producción'
+            ELSE 'Otro'
+        END AS tipo_ticket
+    FROM proyecto.proyecto p
+    JOIN proyecto.ticket t ON 
+        (t.asunto LIKE '%[' || p.codigo || ']%' OR t.asunto LIKE '%' || p.codigo || '%')
+    WHERE p.estado = 'Finalizado'
+),
+ticket_summary AS (
+    SELECT 
+        proyecto_codigo,
+        proyecto_nombre,
+        COUNT(*) AS total_tickets,
+        COUNT(CASE WHEN tipo_ticket = 'Historias de Usuario' THEN 1 END) AS has_historias,
+        COUNT(CASE WHEN tipo_ticket = 'Pruebas de Calidad' THEN 1 END) AS has_pruebas_calidad,
+        COUNT(CASE WHEN tipo_ticket = 'Pruebas de Usuario' THEN 1 END) AS has_pruebas_usuario,
+        COUNT(CASE WHEN tipo_ticket = 'Pase a Producción' THEN 1 END) AS has_pase_produccion,
+        CASE 
+            WHEN COUNT(*) = 4 AND
+                 COUNT(CASE WHEN tipo_ticket = 'Historias de Usuario' THEN 1 END) = 1 AND
+                 COUNT(CASE WHEN tipo_ticket = 'Pruebas de Calidad' THEN 1 END) = 1 AND
+                 COUNT(CASE WHEN tipo_ticket = 'Pruebas de Usuario' THEN 1 END) = 1 AND
+                 COUNT(CASE WHEN tipo_ticket = 'Pase a Producción' THEN 1 END) = 1 
+            THEN 'OK'
+            ELSE 'Faltan tickets'
+        END AS estado_verificacion,
+        STRING_AGG(
+            'ID: ' || ticket_id || ' | Asunto: ' || asunto,
+            ' | ' ORDER BY 
+                CASE tipo_ticket
+                    WHEN 'Historias de Usuario' THEN 1
+                    WHEN 'Pruebas de Calidad' THEN 2
+                    WHEN 'Pruebas de Usuario' THEN 3
+                    WHEN 'Pase a Producción' THEN 4
+                    ELSE 5
+                END
+        ) AS tickets_agrupados
+    FROM project_tickets
+    GROUP BY proyecto_codigo, proyecto_nombre
+)
+SELECT 
+    proyecto_codigo AS "Código Proyecto",
+    proyecto_nombre AS "Nombre Proyecto",
+    total_tickets AS "Total Tickets",
+    estado_verificacion AS "Estado Verificación",
+    CASE WHEN has_historias = 1 THEN '✓' ELSE '✗' END AS "Historias Usuario",
+    CASE WHEN has_pruebas_calidad = 1 THEN '✓' ELSE '✗' END AS "Pruebas Calidad",
+    CASE WHEN has_pruebas_usuario = 1 THEN '✓' ELSE '✗' END AS "Pruebas Usuario",
+    CASE WHEN has_pase_produccion = 1 THEN '✓' ELSE '✗' END AS "Pase Producción",
+    tickets_agrupados AS "Detalle Tickets"
+FROM ticket_summary
+WHERE total_tickets &lt; 4
+ORDER BY proyecto_codigo;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4 -  Documentación de inconsistencias:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Se detecta una inconsistencia en la información de la base de datos, pues se está incumpliendo el diseño establecido en los procedimientos. Esto va en contra de las normas de la empresa y podría generar inconsistencias. Se recomienda comprobar el estado del proceso del ticket que falta, si hace falta terminarlo, y posteriormente ingresarlo a la base de datos; al mismo tiempo, se recomienda cambiar el estado del proyecto de "Finalizado" a "En proceso".</t>
+    </r>
+  </si>
+  <si>
+    <t>Se identificó una leyenda en la columna "asunto", de la tabla "ticket" del esquema "proyecto" de la base de datos "ISW1012_2025" que no cumple con las normas establecidas en el diseño de formato [&lt;codigo de proyecto&gt;]Pruebas de usuario. Se incluían paréntesis redondos en lugar de corchetes en el ticket de id 1003.</t>
+  </si>
+  <si>
+    <t>Incumplimiento de las normas establecidas en el diseño a la hora de ingresar datos a la base de datos. Puede ser por un error en la redacción o por falta de conocimiento de las reglas de nomenclatura por parte de los desarrolladores.</t>
+  </si>
+  <si>
+    <t>Dificultad en la búsqueda de tickets de prueba de calidad.
+Incumplimiento de los estándares de diseño del sistema.
+Incremento en la complejidad del mantenimiento de la base de datos.</t>
+  </si>
+  <si>
+    <t>1. Renombrar el asunto actual para que vaya acorde a las reglas de nomenclatura.
+2. Alterar la sección en donde se ingresen los datos para dejar en claro la nomenclatura establecida y permitir sólo datos válidos con formato [&lt;codigo de proyecto&gt;]Pruebas de usuario.
+3. Realizar auditorías periódicas para asegurar el cumplimiento de los estándares de nomenclatura.</t>
+  </si>
+  <si>
+    <t>De los dos proyectos finalizados registrados en la tabla "proyecto" del esquema "proyecto" de la base de datos "ISW1012_2025", uno de ellos, de código PRY-002 no cuenta con los 4 tiquetes registrados en la tabla "ticket" que debería de tener según el diseño, específicamente, falta el de Pruebas de Usuario.</t>
+  </si>
+  <si>
+    <t>El proceso correspondiente a Pruebas de Usuario no se ha realizado o no se ha registrado el tiquete correctamente según lo estipula el diseño.</t>
+  </si>
+  <si>
+    <t>Inconsistencias en la creación de reportes.
+Pérdida de calidad para los proyectos ubicados en producción.
+Incumplimiento de los estándares y reglas de negocio de la empresa.
+Fallas en el sistema por la falta de las pruebas de usuario.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Sacar el proyecto Mejoras Sistema Financiero, de código PRY-002 de la lista de proyectos finalizados.
+2. Ingresar el ticket faltante manteniendo las reglas de nomenclatura en mente.
+3. Realizar las pruebas de usuario si es que no sólo no fue registrado el ticket, sino que tampoco se hicieron.
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">3 - Análisis de Información:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Se obtuvo que de los dos proyectos finalizados registrados en la tabla "proyecto", uno de ellos, de código PRY-002 contaba con 3 de los 4 tickets requeridos, faltando el de pruebas de usuario.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Se adjunta resultado obtenido Referencia 002</t>
     </r>
   </si>
 </sst>
@@ -878,7 +1010,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -986,6 +1118,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -995,63 +1154,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1122,20 +1225,20 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>57355</xdr:rowOff>
+      <xdr:rowOff>16387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>9007621</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>8193</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>144113</xdr:rowOff>
+      <xdr:rowOff>7608</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{051A8B81-A6F2-3660-DCBC-38CD51B78D42}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F4BF043-91B0-DBB2-35C3-F06E98D4BDD0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1151,8 +1254,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1581355" y="5506065"/>
-          <a:ext cx="9007621" cy="807790"/>
+          <a:off x="1581355" y="10487742"/>
+          <a:ext cx="9029290" cy="712253"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1556775</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>32775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>8988322</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171202</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B251B212-403F-6FCE-65C0-BCBA30DF3367}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1556775" y="22417549"/>
+          <a:ext cx="9012902" cy="679202"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1530,7 +1677,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C5" s="24">
         <v>20</v>
@@ -1541,7 +1688,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C6" s="19">
         <v>40</v>
@@ -1552,7 +1699,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C7" s="22">
         <v>40</v>
@@ -1601,7 +1748,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1626,7 +1773,9 @@
       <c r="A2" s="23">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="C2" s="5" t="s">
         <v>95</v>
       </c>
@@ -1635,7 +1784,9 @@
       <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="C3" s="5" t="s">
         <v>96</v>
       </c>
@@ -1655,66 +1806,53 @@
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="56"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="48"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="48"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="48"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="48"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="48"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="48"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="48"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="62"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="25"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="48"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="48"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1725,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{163B25E8-3DD5-4482-B203-E7A7FE8189D0}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1773,9 +1911,7 @@
       <c r="E2" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="25">
-        <v>1</v>
-      </c>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
@@ -1793,9 +1929,7 @@
       <c r="E3" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="25">
-        <v>2</v>
-      </c>
+      <c r="F3" s="25"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
@@ -1810,68 +1944,64 @@
       <c r="D4" s="31">
         <v>2</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="25"/>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="31">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="45" t="s">
+      <c r="E5" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="25"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B6" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C6" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="46">
-        <v>3</v>
-      </c>
-      <c r="E5" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="25"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="45" t="s">
+      <c r="D6" s="31">
+        <v>4</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="25"/>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B7" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C7" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="46">
-        <v>4</v>
-      </c>
-      <c r="E6" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="25"/>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="46">
+      <c r="D7" s="31">
         <v>5</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="25">
-        <v>4</v>
-      </c>
+      <c r="F7" s="25"/>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
@@ -1889,9 +2019,7 @@
       <c r="E8" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="32">
-        <v>5</v>
-      </c>
+      <c r="F8" s="32"/>
     </row>
     <row r="9" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="28" t="s">
@@ -1906,12 +2034,10 @@
       <c r="D9" s="29">
         <v>1</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="F9" s="32">
-        <v>6</v>
-      </c>
+      <c r="F9" s="32"/>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
@@ -1929,9 +2055,7 @@
       <c r="E10" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="32">
-        <v>7</v>
-      </c>
+      <c r="F10" s="32"/>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="28" t="s">
@@ -1946,12 +2070,10 @@
       <c r="D11" s="29">
         <v>2</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="32">
-        <v>8</v>
-      </c>
+      <c r="F11" s="32"/>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
@@ -1969,9 +2091,7 @@
       <c r="E12" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="32">
-        <v>9</v>
-      </c>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="28" t="s">
@@ -1986,12 +2106,10 @@
       <c r="D13" s="29">
         <v>4</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="32">
-        <v>10</v>
-      </c>
+      <c r="F13" s="32"/>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
@@ -2006,12 +2124,10 @@
       <c r="D14" s="31">
         <v>1</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="25">
-        <v>11</v>
-      </c>
+      <c r="F14" s="25"/>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
@@ -2026,12 +2142,10 @@
       <c r="D15" s="29">
         <v>1</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="25">
-        <v>12</v>
-      </c>
+      <c r="F15" s="25"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
@@ -2046,12 +2160,10 @@
       <c r="D16" s="31">
         <v>1</v>
       </c>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="25">
-        <v>13</v>
-      </c>
+      <c r="F16" s="25"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
@@ -2066,12 +2178,10 @@
       <c r="D17" s="29">
         <v>2</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="25">
-        <v>14</v>
-      </c>
+      <c r="F17" s="25"/>
     </row>
     <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="26" t="s">
@@ -2086,12 +2196,10 @@
       <c r="D18" s="27">
         <v>3</v>
       </c>
-      <c r="E18" s="44" t="s">
+      <c r="E18" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="25">
-        <v>15</v>
-      </c>
+      <c r="F18" s="25"/>
     </row>
     <row r="19" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25"/>
@@ -2191,8 +2299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB44A6A-0034-4084-A496-8529D30A0932}">
   <dimension ref="A2:F427"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="93" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScale="93" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2203,10 +2311,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="51"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
@@ -2229,7 +2337,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="15">
-        <v>45745</v>
+        <v>45747</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2285,7 +2393,7 @@
       <c r="B12" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="57"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
@@ -2309,35 +2417,35 @@
       <c r="A16" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="63" t="s">
-        <v>104</v>
-      </c>
-      <c r="F16" s="62"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="25"/>
+    </row>
+    <row r="17" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
-      <c r="B17" s="63" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B17" s="48" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
-      <c r="B18" s="63" t="s">
-        <v>113</v>
+      <c r="B18" s="47" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
-      <c r="B19" s="64" t="s">
-        <v>115</v>
+      <c r="B19" s="48" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="63" t="s">
-        <v>114</v>
+      <c r="B20" s="47" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -2369,10 +2477,10 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="40"/>
+      <c r="B28" s="51"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
@@ -2395,7 +2503,7 @@
         <v>12</v>
       </c>
       <c r="B31" s="15">
-        <v>45746</v>
+        <v>45747</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -2470,36 +2578,38 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="63" t="s">
-        <v>98</v>
+      <c r="B42" s="47" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A43" s="11"/>
-      <c r="B43" s="63" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B43" s="47" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A44" s="11"/>
-      <c r="B44" s="63" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B44" s="47" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="11"/>
-      <c r="B45" s="64" t="s">
-        <v>101</v>
+      <c r="B45" s="48" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="11"/>
-      <c r="B46" s="63" t="s">
-        <v>102</v>
+      <c r="A46" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="47" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -2507,9 +2617,7 @@
       <c r="B47" s="10"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="11" t="s">
-        <v>5</v>
-      </c>
+      <c r="A48" s="11"/>
       <c r="B48" s="10"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -2533,10 +2641,10 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="39" t="s">
+      <c r="A55" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="B55" s="40"/>
+      <c r="B55" s="51"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
@@ -2665,10 +2773,10 @@
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="39" t="s">
+      <c r="A81" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="B81" s="40"/>
+      <c r="B81" s="51"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="11" t="s">
@@ -2801,1302 +2909,1302 @@
       <c r="B107" s="49"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="50"/>
-      <c r="B108" s="51"/>
+      <c r="A108" s="39"/>
+      <c r="B108" s="40"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="50"/>
-      <c r="B109" s="51"/>
+      <c r="A109" s="39"/>
+      <c r="B109" s="40"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" s="50"/>
-      <c r="B110" s="52"/>
+      <c r="A110" s="39"/>
+      <c r="B110" s="41"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="50"/>
-      <c r="B111" s="51"/>
+      <c r="A111" s="39"/>
+      <c r="B111" s="40"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" s="50"/>
-      <c r="B112" s="51"/>
+      <c r="A112" s="39"/>
+      <c r="B112" s="40"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="50"/>
-      <c r="B113" s="51"/>
+      <c r="A113" s="39"/>
+      <c r="B113" s="40"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" s="50"/>
-      <c r="B114" s="53"/>
+      <c r="A114" s="39"/>
+      <c r="B114" s="42"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="50"/>
-      <c r="B115" s="54"/>
+      <c r="A115" s="39"/>
+      <c r="B115" s="43"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="50"/>
-      <c r="B116" s="51"/>
+      <c r="A116" s="39"/>
+      <c r="B116" s="40"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="50"/>
-      <c r="B117" s="51"/>
+      <c r="A117" s="39"/>
+      <c r="B117" s="40"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="50"/>
-      <c r="B118" s="51"/>
+      <c r="A118" s="39"/>
+      <c r="B118" s="40"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="50"/>
-      <c r="B119" s="51"/>
+      <c r="A119" s="39"/>
+      <c r="B119" s="40"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="50"/>
-      <c r="B120" s="51"/>
+      <c r="A120" s="39"/>
+      <c r="B120" s="40"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="50"/>
-      <c r="B121" s="51"/>
+      <c r="A121" s="39"/>
+      <c r="B121" s="40"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="50"/>
-      <c r="B122" s="51"/>
+      <c r="A122" s="39"/>
+      <c r="B122" s="40"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" s="50"/>
-      <c r="B123" s="51"/>
+      <c r="A123" s="39"/>
+      <c r="B123" s="40"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="50"/>
-      <c r="B124" s="51"/>
+      <c r="A124" s="39"/>
+      <c r="B124" s="40"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="50"/>
-      <c r="B125" s="51"/>
+      <c r="A125" s="39"/>
+      <c r="B125" s="40"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" s="50"/>
-      <c r="B126" s="51"/>
+      <c r="A126" s="39"/>
+      <c r="B126" s="40"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" s="50"/>
-      <c r="B127" s="51"/>
+      <c r="A127" s="39"/>
+      <c r="B127" s="40"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" s="50"/>
-      <c r="B128" s="51"/>
+      <c r="A128" s="39"/>
+      <c r="B128" s="40"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="50"/>
-      <c r="B129" s="51"/>
+      <c r="A129" s="39"/>
+      <c r="B129" s="40"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" s="50"/>
-      <c r="B130" s="51"/>
+      <c r="A130" s="39"/>
+      <c r="B130" s="40"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="50"/>
-      <c r="B131" s="51"/>
+      <c r="A131" s="39"/>
+      <c r="B131" s="40"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="53"/>
-      <c r="B132" s="53"/>
+      <c r="A132" s="42"/>
+      <c r="B132" s="42"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="49"/>
       <c r="B133" s="49"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="50"/>
-      <c r="B134" s="51"/>
+      <c r="A134" s="39"/>
+      <c r="B134" s="40"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A135" s="50"/>
-      <c r="B135" s="51"/>
+      <c r="A135" s="39"/>
+      <c r="B135" s="40"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" s="50"/>
-      <c r="B136" s="52"/>
+      <c r="A136" s="39"/>
+      <c r="B136" s="41"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="50"/>
-      <c r="B137" s="51"/>
+      <c r="A137" s="39"/>
+      <c r="B137" s="40"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" s="50"/>
-      <c r="B138" s="51"/>
+      <c r="A138" s="39"/>
+      <c r="B138" s="40"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A139" s="50"/>
-      <c r="B139" s="51"/>
+      <c r="A139" s="39"/>
+      <c r="B139" s="40"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" s="50"/>
-      <c r="B140" s="53"/>
+      <c r="A140" s="39"/>
+      <c r="B140" s="42"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A141" s="50"/>
-      <c r="B141" s="54"/>
+      <c r="A141" s="39"/>
+      <c r="B141" s="43"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A142" s="50"/>
-      <c r="B142" s="51"/>
+      <c r="A142" s="39"/>
+      <c r="B142" s="40"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A143" s="50"/>
-      <c r="B143" s="51"/>
+      <c r="A143" s="39"/>
+      <c r="B143" s="40"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A144" s="50"/>
-      <c r="B144" s="51"/>
+      <c r="A144" s="39"/>
+      <c r="B144" s="40"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A145" s="50"/>
-      <c r="B145" s="51"/>
+      <c r="A145" s="39"/>
+      <c r="B145" s="40"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A146" s="50"/>
-      <c r="B146" s="51"/>
+      <c r="A146" s="39"/>
+      <c r="B146" s="40"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A147" s="50"/>
-      <c r="B147" s="51"/>
+      <c r="A147" s="39"/>
+      <c r="B147" s="40"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A148" s="50"/>
-      <c r="B148" s="51"/>
+      <c r="A148" s="39"/>
+      <c r="B148" s="40"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A149" s="50"/>
-      <c r="B149" s="51"/>
+      <c r="A149" s="39"/>
+      <c r="B149" s="40"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A150" s="50"/>
-      <c r="B150" s="51"/>
+      <c r="A150" s="39"/>
+      <c r="B150" s="40"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A151" s="50"/>
-      <c r="B151" s="51"/>
+      <c r="A151" s="39"/>
+      <c r="B151" s="40"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A152" s="50"/>
-      <c r="B152" s="51"/>
+      <c r="A152" s="39"/>
+      <c r="B152" s="40"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A153" s="50"/>
-      <c r="B153" s="51"/>
+      <c r="A153" s="39"/>
+      <c r="B153" s="40"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A154" s="50"/>
-      <c r="B154" s="51"/>
+      <c r="A154" s="39"/>
+      <c r="B154" s="40"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A155" s="50"/>
-      <c r="B155" s="51"/>
+      <c r="A155" s="39"/>
+      <c r="B155" s="40"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A156" s="50"/>
-      <c r="B156" s="51"/>
+      <c r="A156" s="39"/>
+      <c r="B156" s="40"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A157" s="50"/>
-      <c r="B157" s="51"/>
+      <c r="A157" s="39"/>
+      <c r="B157" s="40"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A158" s="50"/>
-      <c r="B158" s="51"/>
+      <c r="A158" s="39"/>
+      <c r="B158" s="40"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A159" s="53"/>
-      <c r="B159" s="53"/>
+      <c r="A159" s="42"/>
+      <c r="B159" s="42"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="49"/>
       <c r="B160" s="49"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A161" s="50"/>
-      <c r="B161" s="51"/>
+      <c r="A161" s="39"/>
+      <c r="B161" s="40"/>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A162" s="50"/>
-      <c r="B162" s="51"/>
+      <c r="A162" s="39"/>
+      <c r="B162" s="40"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A163" s="50"/>
-      <c r="B163" s="52"/>
+      <c r="A163" s="39"/>
+      <c r="B163" s="41"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A164" s="50"/>
-      <c r="B164" s="51"/>
+      <c r="A164" s="39"/>
+      <c r="B164" s="40"/>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A165" s="50"/>
-      <c r="B165" s="51"/>
+      <c r="A165" s="39"/>
+      <c r="B165" s="40"/>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A166" s="50"/>
-      <c r="B166" s="51"/>
+      <c r="A166" s="39"/>
+      <c r="B166" s="40"/>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A167" s="50"/>
-      <c r="B167" s="53"/>
+      <c r="A167" s="39"/>
+      <c r="B167" s="42"/>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A168" s="50"/>
-      <c r="B168" s="54"/>
+      <c r="A168" s="39"/>
+      <c r="B168" s="43"/>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A169" s="50"/>
-      <c r="B169" s="51"/>
+      <c r="A169" s="39"/>
+      <c r="B169" s="40"/>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A170" s="50"/>
-      <c r="B170" s="51"/>
+      <c r="A170" s="39"/>
+      <c r="B170" s="40"/>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A171" s="50"/>
-      <c r="B171" s="51"/>
+      <c r="A171" s="39"/>
+      <c r="B171" s="40"/>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A172" s="50"/>
-      <c r="B172" s="51"/>
+      <c r="A172" s="39"/>
+      <c r="B172" s="40"/>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A173" s="50"/>
-      <c r="B173" s="51"/>
+      <c r="A173" s="39"/>
+      <c r="B173" s="40"/>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A174" s="50"/>
-      <c r="B174" s="51"/>
+      <c r="A174" s="39"/>
+      <c r="B174" s="40"/>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A175" s="50"/>
-      <c r="B175" s="51"/>
+      <c r="A175" s="39"/>
+      <c r="B175" s="40"/>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A176" s="50"/>
-      <c r="B176" s="51"/>
+      <c r="A176" s="39"/>
+      <c r="B176" s="40"/>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A177" s="50"/>
-      <c r="B177" s="51"/>
+      <c r="A177" s="39"/>
+      <c r="B177" s="40"/>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A178" s="50"/>
-      <c r="B178" s="51"/>
+      <c r="A178" s="39"/>
+      <c r="B178" s="40"/>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A179" s="50"/>
-      <c r="B179" s="51"/>
+      <c r="A179" s="39"/>
+      <c r="B179" s="40"/>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A180" s="50"/>
-      <c r="B180" s="51"/>
+      <c r="A180" s="39"/>
+      <c r="B180" s="40"/>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A181" s="50"/>
-      <c r="B181" s="51"/>
+      <c r="A181" s="39"/>
+      <c r="B181" s="40"/>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A182" s="50"/>
-      <c r="B182" s="51"/>
+      <c r="A182" s="39"/>
+      <c r="B182" s="40"/>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A183" s="50"/>
-      <c r="B183" s="51"/>
+      <c r="A183" s="39"/>
+      <c r="B183" s="40"/>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A184" s="50"/>
-      <c r="B184" s="51"/>
+      <c r="A184" s="39"/>
+      <c r="B184" s="40"/>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A185" s="53"/>
-      <c r="B185" s="53"/>
+      <c r="A185" s="42"/>
+      <c r="B185" s="42"/>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="49"/>
       <c r="B186" s="49"/>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A187" s="50"/>
-      <c r="B187" s="51"/>
+      <c r="A187" s="39"/>
+      <c r="B187" s="40"/>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A188" s="50"/>
-      <c r="B188" s="51"/>
+      <c r="A188" s="39"/>
+      <c r="B188" s="40"/>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A189" s="50"/>
-      <c r="B189" s="52"/>
+      <c r="A189" s="39"/>
+      <c r="B189" s="41"/>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A190" s="50"/>
-      <c r="B190" s="51"/>
+      <c r="A190" s="39"/>
+      <c r="B190" s="40"/>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A191" s="50"/>
-      <c r="B191" s="51"/>
+      <c r="A191" s="39"/>
+      <c r="B191" s="40"/>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A192" s="50"/>
-      <c r="B192" s="51"/>
+      <c r="A192" s="39"/>
+      <c r="B192" s="40"/>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A193" s="50"/>
-      <c r="B193" s="53"/>
+      <c r="A193" s="39"/>
+      <c r="B193" s="42"/>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A194" s="50"/>
-      <c r="B194" s="54"/>
+      <c r="A194" s="39"/>
+      <c r="B194" s="43"/>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A195" s="50"/>
-      <c r="B195" s="51"/>
+      <c r="A195" s="39"/>
+      <c r="B195" s="40"/>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A196" s="50"/>
-      <c r="B196" s="51"/>
+      <c r="A196" s="39"/>
+      <c r="B196" s="40"/>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A197" s="50"/>
-      <c r="B197" s="51"/>
+      <c r="A197" s="39"/>
+      <c r="B197" s="40"/>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A198" s="50"/>
-      <c r="B198" s="51"/>
+      <c r="A198" s="39"/>
+      <c r="B198" s="40"/>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A199" s="50"/>
-      <c r="B199" s="51"/>
+      <c r="A199" s="39"/>
+      <c r="B199" s="40"/>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A200" s="50"/>
-      <c r="B200" s="51"/>
+      <c r="A200" s="39"/>
+      <c r="B200" s="40"/>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A201" s="50"/>
-      <c r="B201" s="51"/>
+      <c r="A201" s="39"/>
+      <c r="B201" s="40"/>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A202" s="50"/>
-      <c r="B202" s="51"/>
+      <c r="A202" s="39"/>
+      <c r="B202" s="40"/>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A203" s="50"/>
-      <c r="B203" s="51"/>
+      <c r="A203" s="39"/>
+      <c r="B203" s="40"/>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A204" s="50"/>
-      <c r="B204" s="51"/>
+      <c r="A204" s="39"/>
+      <c r="B204" s="40"/>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A205" s="50"/>
-      <c r="B205" s="51"/>
+      <c r="A205" s="39"/>
+      <c r="B205" s="40"/>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A206" s="50"/>
-      <c r="B206" s="51"/>
+      <c r="A206" s="39"/>
+      <c r="B206" s="40"/>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A207" s="50"/>
-      <c r="B207" s="51"/>
+      <c r="A207" s="39"/>
+      <c r="B207" s="40"/>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A208" s="50"/>
-      <c r="B208" s="51"/>
+      <c r="A208" s="39"/>
+      <c r="B208" s="40"/>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A209" s="50"/>
-      <c r="B209" s="51"/>
+      <c r="A209" s="39"/>
+      <c r="B209" s="40"/>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A210" s="50"/>
-      <c r="B210" s="51"/>
+      <c r="A210" s="39"/>
+      <c r="B210" s="40"/>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A211" s="53"/>
-      <c r="B211" s="53"/>
+      <c r="A211" s="42"/>
+      <c r="B211" s="42"/>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" s="49"/>
       <c r="B212" s="49"/>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A213" s="50"/>
-      <c r="B213" s="51"/>
+      <c r="A213" s="39"/>
+      <c r="B213" s="40"/>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A214" s="50"/>
-      <c r="B214" s="51"/>
+      <c r="A214" s="39"/>
+      <c r="B214" s="40"/>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A215" s="50"/>
-      <c r="B215" s="52"/>
+      <c r="A215" s="39"/>
+      <c r="B215" s="41"/>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A216" s="50"/>
-      <c r="B216" s="51"/>
+      <c r="A216" s="39"/>
+      <c r="B216" s="40"/>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A217" s="50"/>
-      <c r="B217" s="51"/>
+      <c r="A217" s="39"/>
+      <c r="B217" s="40"/>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A218" s="50"/>
-      <c r="B218" s="51"/>
+      <c r="A218" s="39"/>
+      <c r="B218" s="40"/>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A219" s="50"/>
-      <c r="B219" s="53"/>
+      <c r="A219" s="39"/>
+      <c r="B219" s="42"/>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A220" s="50"/>
-      <c r="B220" s="54"/>
+      <c r="A220" s="39"/>
+      <c r="B220" s="43"/>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A221" s="50"/>
-      <c r="B221" s="51"/>
+      <c r="A221" s="39"/>
+      <c r="B221" s="40"/>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A222" s="50"/>
-      <c r="B222" s="51"/>
+      <c r="A222" s="39"/>
+      <c r="B222" s="40"/>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A223" s="50"/>
-      <c r="B223" s="51"/>
+      <c r="A223" s="39"/>
+      <c r="B223" s="40"/>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A224" s="50"/>
-      <c r="B224" s="51"/>
+      <c r="A224" s="39"/>
+      <c r="B224" s="40"/>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A225" s="50"/>
-      <c r="B225" s="51"/>
+      <c r="A225" s="39"/>
+      <c r="B225" s="40"/>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A226" s="50"/>
-      <c r="B226" s="51"/>
+      <c r="A226" s="39"/>
+      <c r="B226" s="40"/>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A227" s="50"/>
-      <c r="B227" s="51"/>
+      <c r="A227" s="39"/>
+      <c r="B227" s="40"/>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A228" s="50"/>
-      <c r="B228" s="51"/>
+      <c r="A228" s="39"/>
+      <c r="B228" s="40"/>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A229" s="50"/>
-      <c r="B229" s="51"/>
+      <c r="A229" s="39"/>
+      <c r="B229" s="40"/>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A230" s="50"/>
-      <c r="B230" s="51"/>
+      <c r="A230" s="39"/>
+      <c r="B230" s="40"/>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A231" s="50"/>
-      <c r="B231" s="51"/>
+      <c r="A231" s="39"/>
+      <c r="B231" s="40"/>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A232" s="50"/>
-      <c r="B232" s="51"/>
+      <c r="A232" s="39"/>
+      <c r="B232" s="40"/>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A233" s="50"/>
-      <c r="B233" s="51"/>
+      <c r="A233" s="39"/>
+      <c r="B233" s="40"/>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A234" s="50"/>
-      <c r="B234" s="51"/>
+      <c r="A234" s="39"/>
+      <c r="B234" s="40"/>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A235" s="50"/>
-      <c r="B235" s="51"/>
+      <c r="A235" s="39"/>
+      <c r="B235" s="40"/>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A236" s="50"/>
-      <c r="B236" s="51"/>
+      <c r="A236" s="39"/>
+      <c r="B236" s="40"/>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A237" s="50"/>
-      <c r="B237" s="51"/>
+      <c r="A237" s="39"/>
+      <c r="B237" s="40"/>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A238" s="50"/>
-      <c r="B238" s="51"/>
+      <c r="A238" s="39"/>
+      <c r="B238" s="40"/>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A239" s="53"/>
-      <c r="B239" s="53"/>
+      <c r="A239" s="42"/>
+      <c r="B239" s="42"/>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" s="49"/>
       <c r="B240" s="49"/>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A241" s="50"/>
-      <c r="B241" s="51"/>
+      <c r="A241" s="39"/>
+      <c r="B241" s="40"/>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A242" s="50"/>
-      <c r="B242" s="51"/>
+      <c r="A242" s="39"/>
+      <c r="B242" s="40"/>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A243" s="50"/>
-      <c r="B243" s="52"/>
+      <c r="A243" s="39"/>
+      <c r="B243" s="41"/>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A244" s="50"/>
-      <c r="B244" s="51"/>
+      <c r="A244" s="39"/>
+      <c r="B244" s="40"/>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A245" s="50"/>
-      <c r="B245" s="51"/>
+      <c r="A245" s="39"/>
+      <c r="B245" s="40"/>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A246" s="50"/>
-      <c r="B246" s="51"/>
+      <c r="A246" s="39"/>
+      <c r="B246" s="40"/>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A247" s="50"/>
-      <c r="B247" s="53"/>
+      <c r="A247" s="39"/>
+      <c r="B247" s="42"/>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A248" s="50"/>
-      <c r="B248" s="54"/>
+      <c r="A248" s="39"/>
+      <c r="B248" s="43"/>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A249" s="50"/>
-      <c r="B249" s="51"/>
+      <c r="A249" s="39"/>
+      <c r="B249" s="40"/>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A250" s="50"/>
-      <c r="B250" s="51"/>
+      <c r="A250" s="39"/>
+      <c r="B250" s="40"/>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A251" s="50"/>
-      <c r="B251" s="51"/>
+      <c r="A251" s="39"/>
+      <c r="B251" s="40"/>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A252" s="50"/>
-      <c r="B252" s="51"/>
+      <c r="A252" s="39"/>
+      <c r="B252" s="40"/>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A253" s="50"/>
-      <c r="B253" s="51"/>
+      <c r="A253" s="39"/>
+      <c r="B253" s="40"/>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A254" s="50"/>
-      <c r="B254" s="51"/>
+      <c r="A254" s="39"/>
+      <c r="B254" s="40"/>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A255" s="50"/>
-      <c r="B255" s="51"/>
+      <c r="A255" s="39"/>
+      <c r="B255" s="40"/>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A256" s="50"/>
-      <c r="B256" s="51"/>
+      <c r="A256" s="39"/>
+      <c r="B256" s="40"/>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A257" s="50"/>
-      <c r="B257" s="51"/>
+      <c r="A257" s="39"/>
+      <c r="B257" s="40"/>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A258" s="50"/>
-      <c r="B258" s="51"/>
+      <c r="A258" s="39"/>
+      <c r="B258" s="40"/>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A259" s="50"/>
-      <c r="B259" s="51"/>
+      <c r="A259" s="39"/>
+      <c r="B259" s="40"/>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A260" s="50"/>
-      <c r="B260" s="51"/>
+      <c r="A260" s="39"/>
+      <c r="B260" s="40"/>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A261" s="50"/>
-      <c r="B261" s="51"/>
+      <c r="A261" s="39"/>
+      <c r="B261" s="40"/>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A262" s="50"/>
-      <c r="B262" s="51"/>
+      <c r="A262" s="39"/>
+      <c r="B262" s="40"/>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A263" s="50"/>
-      <c r="B263" s="51"/>
+      <c r="A263" s="39"/>
+      <c r="B263" s="40"/>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A264" s="50"/>
-      <c r="B264" s="51"/>
+      <c r="A264" s="39"/>
+      <c r="B264" s="40"/>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A265" s="53"/>
-      <c r="B265" s="53"/>
+      <c r="A265" s="42"/>
+      <c r="B265" s="42"/>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" s="49"/>
       <c r="B266" s="49"/>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A267" s="50"/>
-      <c r="B267" s="51"/>
+      <c r="A267" s="39"/>
+      <c r="B267" s="40"/>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A268" s="50"/>
-      <c r="B268" s="51"/>
+      <c r="A268" s="39"/>
+      <c r="B268" s="40"/>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A269" s="50"/>
-      <c r="B269" s="52"/>
+      <c r="A269" s="39"/>
+      <c r="B269" s="41"/>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A270" s="50"/>
-      <c r="B270" s="51"/>
+      <c r="A270" s="39"/>
+      <c r="B270" s="40"/>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A271" s="50"/>
-      <c r="B271" s="51"/>
+      <c r="A271" s="39"/>
+      <c r="B271" s="40"/>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A272" s="50"/>
-      <c r="B272" s="51"/>
+      <c r="A272" s="39"/>
+      <c r="B272" s="40"/>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A273" s="50"/>
-      <c r="B273" s="53"/>
+      <c r="A273" s="39"/>
+      <c r="B273" s="42"/>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A274" s="50"/>
-      <c r="B274" s="54"/>
+      <c r="A274" s="39"/>
+      <c r="B274" s="43"/>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A275" s="50"/>
-      <c r="B275" s="51"/>
+      <c r="A275" s="39"/>
+      <c r="B275" s="40"/>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A276" s="50"/>
-      <c r="B276" s="51"/>
+      <c r="A276" s="39"/>
+      <c r="B276" s="40"/>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A277" s="50"/>
-      <c r="B277" s="51"/>
+      <c r="A277" s="39"/>
+      <c r="B277" s="40"/>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A278" s="50"/>
-      <c r="B278" s="51"/>
+      <c r="A278" s="39"/>
+      <c r="B278" s="40"/>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A279" s="50"/>
-      <c r="B279" s="51"/>
+      <c r="A279" s="39"/>
+      <c r="B279" s="40"/>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A280" s="50"/>
-      <c r="B280" s="51"/>
+      <c r="A280" s="39"/>
+      <c r="B280" s="40"/>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A281" s="50"/>
-      <c r="B281" s="51"/>
+      <c r="A281" s="39"/>
+      <c r="B281" s="40"/>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A282" s="50"/>
-      <c r="B282" s="51"/>
+      <c r="A282" s="39"/>
+      <c r="B282" s="40"/>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A283" s="50"/>
-      <c r="B283" s="51"/>
+      <c r="A283" s="39"/>
+      <c r="B283" s="40"/>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A284" s="50"/>
-      <c r="B284" s="51"/>
+      <c r="A284" s="39"/>
+      <c r="B284" s="40"/>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A285" s="50"/>
-      <c r="B285" s="51"/>
+      <c r="A285" s="39"/>
+      <c r="B285" s="40"/>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A286" s="50"/>
-      <c r="B286" s="51"/>
+      <c r="A286" s="39"/>
+      <c r="B286" s="40"/>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A287" s="50"/>
-      <c r="B287" s="51"/>
+      <c r="A287" s="39"/>
+      <c r="B287" s="40"/>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A288" s="50"/>
-      <c r="B288" s="51"/>
+      <c r="A288" s="39"/>
+      <c r="B288" s="40"/>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A289" s="50"/>
-      <c r="B289" s="51"/>
+      <c r="A289" s="39"/>
+      <c r="B289" s="40"/>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A290" s="50"/>
-      <c r="B290" s="51"/>
+      <c r="A290" s="39"/>
+      <c r="B290" s="40"/>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A291" s="53"/>
-      <c r="B291" s="53"/>
+      <c r="A291" s="42"/>
+      <c r="B291" s="42"/>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" s="49"/>
       <c r="B292" s="49"/>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A293" s="50"/>
-      <c r="B293" s="51"/>
+      <c r="A293" s="39"/>
+      <c r="B293" s="40"/>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A294" s="50"/>
-      <c r="B294" s="51"/>
+      <c r="A294" s="39"/>
+      <c r="B294" s="40"/>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A295" s="50"/>
-      <c r="B295" s="52"/>
+      <c r="A295" s="39"/>
+      <c r="B295" s="41"/>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A296" s="50"/>
-      <c r="B296" s="51"/>
+      <c r="A296" s="39"/>
+      <c r="B296" s="40"/>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A297" s="50"/>
-      <c r="B297" s="51"/>
+      <c r="A297" s="39"/>
+      <c r="B297" s="40"/>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A298" s="50"/>
-      <c r="B298" s="51"/>
+      <c r="A298" s="39"/>
+      <c r="B298" s="40"/>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A299" s="50"/>
-      <c r="B299" s="53"/>
+      <c r="A299" s="39"/>
+      <c r="B299" s="42"/>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A300" s="50"/>
-      <c r="B300" s="54"/>
+      <c r="A300" s="39"/>
+      <c r="B300" s="43"/>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A301" s="50"/>
-      <c r="B301" s="51"/>
+      <c r="A301" s="39"/>
+      <c r="B301" s="40"/>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A302" s="50"/>
-      <c r="B302" s="51"/>
+      <c r="A302" s="39"/>
+      <c r="B302" s="40"/>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A303" s="50"/>
-      <c r="B303" s="51"/>
+      <c r="A303" s="39"/>
+      <c r="B303" s="40"/>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A304" s="50"/>
-      <c r="B304" s="51"/>
+      <c r="A304" s="39"/>
+      <c r="B304" s="40"/>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A305" s="50"/>
-      <c r="B305" s="51"/>
+      <c r="A305" s="39"/>
+      <c r="B305" s="40"/>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A306" s="50"/>
-      <c r="B306" s="51"/>
+      <c r="A306" s="39"/>
+      <c r="B306" s="40"/>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A307" s="50"/>
-      <c r="B307" s="51"/>
+      <c r="A307" s="39"/>
+      <c r="B307" s="40"/>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A308" s="50"/>
-      <c r="B308" s="51"/>
+      <c r="A308" s="39"/>
+      <c r="B308" s="40"/>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A309" s="50"/>
-      <c r="B309" s="51"/>
+      <c r="A309" s="39"/>
+      <c r="B309" s="40"/>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A310" s="50"/>
-      <c r="B310" s="51"/>
+      <c r="A310" s="39"/>
+      <c r="B310" s="40"/>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A311" s="50"/>
-      <c r="B311" s="51"/>
+      <c r="A311" s="39"/>
+      <c r="B311" s="40"/>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A312" s="50"/>
-      <c r="B312" s="51"/>
+      <c r="A312" s="39"/>
+      <c r="B312" s="40"/>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A313" s="50"/>
-      <c r="B313" s="51"/>
+      <c r="A313" s="39"/>
+      <c r="B313" s="40"/>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A314" s="50"/>
-      <c r="B314" s="51"/>
+      <c r="A314" s="39"/>
+      <c r="B314" s="40"/>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A315" s="50"/>
-      <c r="B315" s="51"/>
+      <c r="A315" s="39"/>
+      <c r="B315" s="40"/>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A316" s="50"/>
-      <c r="B316" s="51"/>
+      <c r="A316" s="39"/>
+      <c r="B316" s="40"/>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A317" s="53"/>
-      <c r="B317" s="53"/>
+      <c r="A317" s="42"/>
+      <c r="B317" s="42"/>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A318" s="49"/>
       <c r="B318" s="49"/>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A319" s="50"/>
-      <c r="B319" s="51"/>
+      <c r="A319" s="39"/>
+      <c r="B319" s="40"/>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A320" s="50"/>
-      <c r="B320" s="51"/>
+      <c r="A320" s="39"/>
+      <c r="B320" s="40"/>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A321" s="50"/>
-      <c r="B321" s="52"/>
+      <c r="A321" s="39"/>
+      <c r="B321" s="41"/>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A322" s="50"/>
-      <c r="B322" s="51"/>
+      <c r="A322" s="39"/>
+      <c r="B322" s="40"/>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A323" s="50"/>
-      <c r="B323" s="51"/>
+      <c r="A323" s="39"/>
+      <c r="B323" s="40"/>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A324" s="50"/>
-      <c r="B324" s="51"/>
+      <c r="A324" s="39"/>
+      <c r="B324" s="40"/>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A325" s="50"/>
-      <c r="B325" s="53"/>
+      <c r="A325" s="39"/>
+      <c r="B325" s="42"/>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A326" s="50"/>
-      <c r="B326" s="54"/>
+      <c r="A326" s="39"/>
+      <c r="B326" s="43"/>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A327" s="50"/>
-      <c r="B327" s="51"/>
+      <c r="A327" s="39"/>
+      <c r="B327" s="40"/>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A328" s="50"/>
-      <c r="B328" s="51"/>
+      <c r="A328" s="39"/>
+      <c r="B328" s="40"/>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A329" s="50"/>
-      <c r="B329" s="51"/>
+      <c r="A329" s="39"/>
+      <c r="B329" s="40"/>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A330" s="50"/>
-      <c r="B330" s="51"/>
+      <c r="A330" s="39"/>
+      <c r="B330" s="40"/>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A331" s="50"/>
-      <c r="B331" s="51"/>
+      <c r="A331" s="39"/>
+      <c r="B331" s="40"/>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A332" s="50"/>
-      <c r="B332" s="51"/>
+      <c r="A332" s="39"/>
+      <c r="B332" s="40"/>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A333" s="50"/>
-      <c r="B333" s="51"/>
+      <c r="A333" s="39"/>
+      <c r="B333" s="40"/>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A334" s="50"/>
-      <c r="B334" s="51"/>
+      <c r="A334" s="39"/>
+      <c r="B334" s="40"/>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A335" s="50"/>
-      <c r="B335" s="51"/>
+      <c r="A335" s="39"/>
+      <c r="B335" s="40"/>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A336" s="50"/>
-      <c r="B336" s="51"/>
+      <c r="A336" s="39"/>
+      <c r="B336" s="40"/>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A337" s="50"/>
-      <c r="B337" s="51"/>
+      <c r="A337" s="39"/>
+      <c r="B337" s="40"/>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A338" s="50"/>
-      <c r="B338" s="51"/>
+      <c r="A338" s="39"/>
+      <c r="B338" s="40"/>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A339" s="50"/>
-      <c r="B339" s="51"/>
+      <c r="A339" s="39"/>
+      <c r="B339" s="40"/>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A340" s="50"/>
-      <c r="B340" s="51"/>
+      <c r="A340" s="39"/>
+      <c r="B340" s="40"/>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A341" s="50"/>
-      <c r="B341" s="51"/>
+      <c r="A341" s="39"/>
+      <c r="B341" s="40"/>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A342" s="50"/>
-      <c r="B342" s="51"/>
+      <c r="A342" s="39"/>
+      <c r="B342" s="40"/>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A343" s="53"/>
-      <c r="B343" s="53"/>
+      <c r="A343" s="42"/>
+      <c r="B343" s="42"/>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A344" s="49"/>
       <c r="B344" s="49"/>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A345" s="50"/>
-      <c r="B345" s="51"/>
+      <c r="A345" s="39"/>
+      <c r="B345" s="40"/>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A346" s="50"/>
-      <c r="B346" s="51"/>
+      <c r="A346" s="39"/>
+      <c r="B346" s="40"/>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A347" s="50"/>
-      <c r="B347" s="52"/>
+      <c r="A347" s="39"/>
+      <c r="B347" s="41"/>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A348" s="50"/>
-      <c r="B348" s="51"/>
+      <c r="A348" s="39"/>
+      <c r="B348" s="40"/>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A349" s="50"/>
-      <c r="B349" s="51"/>
+      <c r="A349" s="39"/>
+      <c r="B349" s="40"/>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A350" s="50"/>
-      <c r="B350" s="51"/>
+      <c r="A350" s="39"/>
+      <c r="B350" s="40"/>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A351" s="50"/>
-      <c r="B351" s="53"/>
+      <c r="A351" s="39"/>
+      <c r="B351" s="42"/>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A352" s="50"/>
-      <c r="B352" s="54"/>
+      <c r="A352" s="39"/>
+      <c r="B352" s="43"/>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A353" s="50"/>
-      <c r="B353" s="51"/>
+      <c r="A353" s="39"/>
+      <c r="B353" s="40"/>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A354" s="50"/>
-      <c r="B354" s="51"/>
+      <c r="A354" s="39"/>
+      <c r="B354" s="40"/>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A355" s="50"/>
-      <c r="B355" s="51"/>
+      <c r="A355" s="39"/>
+      <c r="B355" s="40"/>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A356" s="50"/>
-      <c r="B356" s="51"/>
+      <c r="A356" s="39"/>
+      <c r="B356" s="40"/>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A357" s="50"/>
-      <c r="B357" s="51"/>
+      <c r="A357" s="39"/>
+      <c r="B357" s="40"/>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A358" s="50"/>
-      <c r="B358" s="51"/>
+      <c r="A358" s="39"/>
+      <c r="B358" s="40"/>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A359" s="50"/>
-      <c r="B359" s="51"/>
+      <c r="A359" s="39"/>
+      <c r="B359" s="40"/>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A360" s="50"/>
-      <c r="B360" s="51"/>
+      <c r="A360" s="39"/>
+      <c r="B360" s="40"/>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A361" s="50"/>
-      <c r="B361" s="51"/>
+      <c r="A361" s="39"/>
+      <c r="B361" s="40"/>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A362" s="50"/>
-      <c r="B362" s="51"/>
+      <c r="A362" s="39"/>
+      <c r="B362" s="40"/>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A363" s="50"/>
-      <c r="B363" s="51"/>
+      <c r="A363" s="39"/>
+      <c r="B363" s="40"/>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A364" s="50"/>
-      <c r="B364" s="51"/>
+      <c r="A364" s="39"/>
+      <c r="B364" s="40"/>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A365" s="50"/>
-      <c r="B365" s="51"/>
+      <c r="A365" s="39"/>
+      <c r="B365" s="40"/>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A366" s="50"/>
-      <c r="B366" s="51"/>
+      <c r="A366" s="39"/>
+      <c r="B366" s="40"/>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A367" s="50"/>
-      <c r="B367" s="51"/>
+      <c r="A367" s="39"/>
+      <c r="B367" s="40"/>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A368" s="50"/>
-      <c r="B368" s="51"/>
+      <c r="A368" s="39"/>
+      <c r="B368" s="40"/>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A369" s="53"/>
-      <c r="B369" s="53"/>
+      <c r="A369" s="42"/>
+      <c r="B369" s="42"/>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A370" s="49"/>
       <c r="B370" s="49"/>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A371" s="50"/>
-      <c r="B371" s="51"/>
+      <c r="A371" s="39"/>
+      <c r="B371" s="40"/>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A372" s="50"/>
-      <c r="B372" s="51"/>
+      <c r="A372" s="39"/>
+      <c r="B372" s="40"/>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A373" s="50"/>
-      <c r="B373" s="52"/>
+      <c r="A373" s="39"/>
+      <c r="B373" s="41"/>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A374" s="50"/>
-      <c r="B374" s="51"/>
+      <c r="A374" s="39"/>
+      <c r="B374" s="40"/>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A375" s="50"/>
-      <c r="B375" s="51"/>
+      <c r="A375" s="39"/>
+      <c r="B375" s="40"/>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A376" s="50"/>
-      <c r="B376" s="51"/>
+      <c r="A376" s="39"/>
+      <c r="B376" s="40"/>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A377" s="50"/>
-      <c r="B377" s="53"/>
+      <c r="A377" s="39"/>
+      <c r="B377" s="42"/>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A378" s="50"/>
-      <c r="B378" s="54"/>
+      <c r="A378" s="39"/>
+      <c r="B378" s="43"/>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A379" s="50"/>
-      <c r="B379" s="51"/>
+      <c r="A379" s="39"/>
+      <c r="B379" s="40"/>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A380" s="50"/>
-      <c r="B380" s="51"/>
+      <c r="A380" s="39"/>
+      <c r="B380" s="40"/>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A381" s="50"/>
-      <c r="B381" s="51"/>
+      <c r="A381" s="39"/>
+      <c r="B381" s="40"/>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A382" s="50"/>
-      <c r="B382" s="51"/>
+      <c r="A382" s="39"/>
+      <c r="B382" s="40"/>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A383" s="50"/>
-      <c r="B383" s="51"/>
+      <c r="A383" s="39"/>
+      <c r="B383" s="40"/>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A384" s="50"/>
-      <c r="B384" s="51"/>
+      <c r="A384" s="39"/>
+      <c r="B384" s="40"/>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A385" s="50"/>
-      <c r="B385" s="51"/>
+      <c r="A385" s="39"/>
+      <c r="B385" s="40"/>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A386" s="50"/>
-      <c r="B386" s="51"/>
+      <c r="A386" s="39"/>
+      <c r="B386" s="40"/>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A387" s="50"/>
-      <c r="B387" s="51"/>
+      <c r="A387" s="39"/>
+      <c r="B387" s="40"/>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A388" s="50"/>
-      <c r="B388" s="51"/>
+      <c r="A388" s="39"/>
+      <c r="B388" s="40"/>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A389" s="50"/>
-      <c r="B389" s="51"/>
+      <c r="A389" s="39"/>
+      <c r="B389" s="40"/>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A390" s="50"/>
-      <c r="B390" s="51"/>
+      <c r="A390" s="39"/>
+      <c r="B390" s="40"/>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A391" s="50"/>
-      <c r="B391" s="51"/>
+      <c r="A391" s="39"/>
+      <c r="B391" s="40"/>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A392" s="50"/>
-      <c r="B392" s="51"/>
+      <c r="A392" s="39"/>
+      <c r="B392" s="40"/>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A393" s="50"/>
-      <c r="B393" s="51"/>
+      <c r="A393" s="39"/>
+      <c r="B393" s="40"/>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A394" s="50"/>
-      <c r="B394" s="51"/>
+      <c r="A394" s="39"/>
+      <c r="B394" s="40"/>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A395" s="53"/>
-      <c r="B395" s="53"/>
+      <c r="A395" s="42"/>
+      <c r="B395" s="42"/>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A396" s="53"/>
-      <c r="B396" s="53"/>
+      <c r="A396" s="42"/>
+      <c r="B396" s="42"/>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A397" s="53"/>
-      <c r="B397" s="53"/>
+      <c r="A397" s="42"/>
+      <c r="B397" s="42"/>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A398" s="53"/>
-      <c r="B398" s="53"/>
+      <c r="A398" s="42"/>
+      <c r="B398" s="42"/>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A399" s="53"/>
-      <c r="B399" s="53"/>
+      <c r="A399" s="42"/>
+      <c r="B399" s="42"/>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A400" s="53"/>
-      <c r="B400" s="53"/>
+      <c r="A400" s="42"/>
+      <c r="B400" s="42"/>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A401" s="53"/>
-      <c r="B401" s="53"/>
+      <c r="A401" s="42"/>
+      <c r="B401" s="42"/>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A402" s="53"/>
-      <c r="B402" s="53"/>
+      <c r="A402" s="42"/>
+      <c r="B402" s="42"/>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A403" s="53"/>
-      <c r="B403" s="53"/>
+      <c r="A403" s="42"/>
+      <c r="B403" s="42"/>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A404" s="53"/>
-      <c r="B404" s="53"/>
+      <c r="A404" s="42"/>
+      <c r="B404" s="42"/>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A405" s="53"/>
-      <c r="B405" s="53"/>
+      <c r="A405" s="42"/>
+      <c r="B405" s="42"/>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A406" s="53"/>
-      <c r="B406" s="53"/>
+      <c r="A406" s="42"/>
+      <c r="B406" s="42"/>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A407" s="53"/>
-      <c r="B407" s="53"/>
+      <c r="A407" s="42"/>
+      <c r="B407" s="42"/>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A408" s="53"/>
-      <c r="B408" s="53"/>
+      <c r="A408" s="42"/>
+      <c r="B408" s="42"/>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A409" s="53"/>
-      <c r="B409" s="53"/>
+      <c r="A409" s="42"/>
+      <c r="B409" s="42"/>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A410" s="53"/>
-      <c r="B410" s="53"/>
+      <c r="A410" s="42"/>
+      <c r="B410" s="42"/>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A411" s="53"/>
-      <c r="B411" s="53"/>
+      <c r="A411" s="42"/>
+      <c r="B411" s="42"/>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A412" s="53"/>
-      <c r="B412" s="53"/>
+      <c r="A412" s="42"/>
+      <c r="B412" s="42"/>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A413" s="53"/>
-      <c r="B413" s="53"/>
+      <c r="A413" s="42"/>
+      <c r="B413" s="42"/>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A414" s="53"/>
-      <c r="B414" s="53"/>
+      <c r="A414" s="42"/>
+      <c r="B414" s="42"/>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A415" s="53"/>
-      <c r="B415" s="53"/>
+      <c r="A415" s="42"/>
+      <c r="B415" s="42"/>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A416" s="53"/>
-      <c r="B416" s="53"/>
+      <c r="A416" s="42"/>
+      <c r="B416" s="42"/>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A417" s="53"/>
-      <c r="B417" s="53"/>
+      <c r="A417" s="42"/>
+      <c r="B417" s="42"/>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A418" s="53"/>
-      <c r="B418" s="53"/>
+      <c r="A418" s="42"/>
+      <c r="B418" s="42"/>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A419" s="53"/>
-      <c r="B419" s="53"/>
+      <c r="A419" s="42"/>
+      <c r="B419" s="42"/>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A420" s="53"/>
-      <c r="B420" s="53"/>
+      <c r="A420" s="42"/>
+      <c r="B420" s="42"/>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A421" s="53"/>
-      <c r="B421" s="53"/>
+      <c r="A421" s="42"/>
+      <c r="B421" s="42"/>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A422" s="53"/>
-      <c r="B422" s="53"/>
+      <c r="A422" s="42"/>
+      <c r="B422" s="42"/>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A423" s="53"/>
-      <c r="B423" s="53"/>
+      <c r="A423" s="42"/>
+      <c r="B423" s="42"/>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A424" s="53"/>
-      <c r="B424" s="53"/>
+      <c r="A424" s="42"/>
+      <c r="B424" s="42"/>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A425" s="53"/>
-      <c r="B425" s="53"/>
+      <c r="A425" s="42"/>
+      <c r="B425" s="42"/>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A426" s="53"/>
-      <c r="B426" s="53"/>
+      <c r="A426" s="42"/>
+      <c r="B426" s="42"/>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A427" s="53"/>
-      <c r="B427" s="53"/>
+      <c r="A427" s="42"/>
+      <c r="B427" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A318:B318"/>
+    <mergeCell ref="A344:B344"/>
+    <mergeCell ref="A370:B370"/>
+    <mergeCell ref="A266:B266"/>
+    <mergeCell ref="A292:B292"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A107:B107"/>
     <mergeCell ref="A133:B133"/>
     <mergeCell ref="A160:B160"/>
     <mergeCell ref="A186:B186"/>
     <mergeCell ref="A212:B212"/>
     <mergeCell ref="A240:B240"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A318:B318"/>
-    <mergeCell ref="A344:B344"/>
-    <mergeCell ref="A370:B370"/>
-    <mergeCell ref="A266:B266"/>
-    <mergeCell ref="A292:B292"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4108,8 +4216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60956F3D-C987-4238-988D-0C3BF01C0F28}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4120,37 +4228,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="41"/>
-    </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B1" s="52"/>
+    </row>
+    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="D2" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="53"/>
+    </row>
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="D3" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="53"/>
+    </row>
+    <row r="4" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="D4" s="5" t="s">
-        <v>110</v>
-      </c>
+      <c r="B4" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="53"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
@@ -4159,43 +4267,47 @@
       <c r="B5" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D5" s="53"/>
+    </row>
+    <row r="6" spans="1:4" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="D6" s="6" t="s">
-        <v>112</v>
-      </c>
+      <c r="B6" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="53"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="41"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="52"/>
+    </row>
+    <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
@@ -4205,18 +4317,20 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="61.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="41"/>
+      <c r="B15" s="52"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
@@ -4250,10 +4364,10 @@
     </row>
     <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="41"/>
+      <c r="B22" s="52"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">

</xml_diff>